<commit_message>
Fully-functional starmap with constellations
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176691" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182490" uniqueCount="286">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -857,6 +857,24 @@
   </si>
   <si>
     <t xml:space="preserve">↓</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go To</t>
   </si>
 </sst>
 </file>
@@ -2215,6 +2233,28 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>269</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8"/>
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2611,7 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
         <v>120</v>
@@ -2583,7 +2623,7 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>280</v>
       </c>
       <c r="G18" t="s">
         <v>120</v>
@@ -2591,7 +2631,7 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -2603,7 +2643,7 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>130</v>
+        <v>280</v>
       </c>
       <c r="G19" t="s">
         <v>40</v>
@@ -2611,7 +2651,7 @@
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -2623,7 +2663,7 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>280</v>
       </c>
       <c r="G20" t="s">
         <v>39</v>
@@ -3494,6 +3534,57 @@
       </c>
       <c r="F71" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>281</v>
+      </c>
+      <c r="C72" t="s">
+        <v>281</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>282</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E73" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>283</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" t="s">
+        <v>47</v>
+      </c>
+      <c r="E74" t="s">
+        <v>43</v>
+      </c>
+      <c r="F74" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working interface with control box.
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182490" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183406" uniqueCount="288">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -875,6 +875,12 @@
   </si>
   <si>
     <t xml:space="preserve">Go To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+00h00'00"E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+00°00'00"N</t>
   </si>
 </sst>
 </file>
@@ -2402,7 +2408,7 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6">
@@ -2436,7 +2442,7 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>191</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
added functions to mount screen
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183406" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186154" uniqueCount="291">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -881,6 +881,15 @@
   </si>
   <si>
     <t xml:space="preserve">+00°00'00"N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;RA&gt;   &lt;DEC&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTC-4 21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTC-4  21:00:00</t>
   </si>
 </sst>
 </file>
@@ -2476,7 +2485,7 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10">
@@ -3057,13 +3066,13 @@
         <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E43" t="s">
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44">
@@ -3125,13 +3134,13 @@
         <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>210</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48">

</xml_diff>

<commit_message>
Implementing new Joystick for nudging
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415724" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436796" uniqueCount="994">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -5223,6 +5223,465 @@
 Dec:
 Altitude:
 Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA Index: %f
+Dec Index: %f
+Cone value: %f
+PA Alt: %f
+PA Az: %f
+Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA: 
+Hour angle: 
+Dec:
+Altitude:
+Magnitude: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save Settings</t>
   </si>
 </sst>
 </file>
@@ -8425,7 +8884,7 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>929</v>
+        <v>795</v>
       </c>
     </row>
     <row r="104">
@@ -8442,7 +8901,24 @@
         <v>43</v>
       </c>
       <c r="F104" t="s">
-        <v>930</v>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>991</v>
+      </c>
+      <c r="C105" t="s">
+        <v>40</v>
+      </c>
+      <c r="D105" t="s">
+        <v>47</v>
+      </c>
+      <c r="E105" t="s">
+        <v>43</v>
+      </c>
+      <c r="F105" t="s">
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
swipe added but not perfected
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523464" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529740" uniqueCount="1237">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6720,6 +6720,30 @@
   <si>
     <t xml:space="preserve">Once aligned, press
 the button below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration er</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration error too </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration error too lar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration error too large. Re-try </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration error too large. Re-try star alignment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration error too large. Re-try star alignment first.</t>
   </si>
 </sst>
 </file>
@@ -9973,7 +9997,7 @@
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>1226</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="107">
@@ -10041,7 +10065,7 @@
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>1227</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="111">
@@ -10058,7 +10082,7 @@
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>1228</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="112">
@@ -10093,6 +10117,23 @@
       </c>
       <c r="F113" t="s">
         <v>1187</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C114" t="s">
+        <v>40</v>
+      </c>
+      <c r="D114" t="s">
+        <v>42</v>
+      </c>
+      <c r="E114" t="s">
+        <v>43</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement slider for slew speed.
BUGS:
1. Axis moving in slow speed has bugs when switching direction quickly from W to E
2. Axis moving in x1 sidereal speed => Crash the controller
</commit_message>
<xml_diff>
--- a/touchgfx/assets/texts/texts.xlsx
+++ b/touchgfx/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529740" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531822" uniqueCount="1238">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6744,6 +6744,9 @@
   </si>
   <si>
     <t xml:space="preserve">Calibration error too large. Re-try star alignment first.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId132</t>
   </si>
 </sst>
 </file>
@@ -9050,7 +9053,7 @@
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C51" t="s">
         <v>120</v>
@@ -9062,63 +9065,63 @@
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E52" t="s">
         <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C53" t="s">
         <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E53" t="s">
         <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>295</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C54" t="s">
-        <v>39</v>
+        <v>262</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E54" t="s">
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="C55" t="s">
         <v>262</v>
@@ -9130,32 +9133,32 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>172</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="C56" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="D56" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E56" t="s">
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C57" t="s">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
@@ -9164,46 +9167,46 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>280</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C58" t="s">
         <v>40</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
       </c>
       <c r="F58" t="s">
-        <v>74</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="D59" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E59" t="s">
         <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>285</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C60" t="s">
         <v>262</v>
@@ -9215,12 +9218,12 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C61" t="s">
         <v>262</v>
@@ -9232,12 +9235,12 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C62" t="s">
         <v>262</v>
@@ -9249,12 +9252,12 @@
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C63" t="s">
         <v>262</v>
@@ -9266,29 +9269,29 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C64" t="s">
-        <v>262</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E64" t="s">
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
@@ -9300,29 +9303,29 @@
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D66" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E66" t="s">
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>144</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C67" t="s">
         <v>120</v>
@@ -9334,12 +9337,12 @@
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C68" t="s">
         <v>120</v>
@@ -9351,12 +9354,12 @@
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C69" t="s">
         <v>120</v>
@@ -9373,7 +9376,7 @@
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C70" t="s">
         <v>120</v>
@@ -9385,12 +9388,12 @@
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C71" t="s">
         <v>120</v>
@@ -9402,12 +9405,12 @@
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C72" t="s">
         <v>120</v>
@@ -9419,12 +9422,12 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C73" t="s">
         <v>120</v>
@@ -9436,12 +9439,12 @@
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C74" t="s">
         <v>120</v>
@@ -9453,12 +9456,12 @@
         <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C75" t="s">
         <v>120</v>
@@ -9470,12 +9473,12 @@
         <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C76" t="s">
         <v>120</v>
@@ -9487,12 +9490,12 @@
         <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C77" t="s">
         <v>120</v>
@@ -9504,83 +9507,83 @@
         <v>43</v>
       </c>
       <c r="F77" t="s">
-        <v>316</v>
+        <v>337</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D78" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E78" t="s">
         <v>43</v>
       </c>
       <c r="F78" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C79" t="s">
         <v>40</v>
       </c>
       <c r="D79" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
         <v>43</v>
       </c>
       <c r="F79" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C80" t="s">
         <v>40</v>
       </c>
       <c r="D80" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E80" t="s">
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C81" t="s">
         <v>40</v>
       </c>
       <c r="D81" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E81" t="s">
         <v>43</v>
       </c>
       <c r="F81" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
         <v>42</v>
@@ -9589,12 +9592,12 @@
         <v>43</v>
       </c>
       <c r="F82" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C83" t="s">
         <v>39</v>
@@ -9606,12 +9609,12 @@
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>316</v>
+        <v>271</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C84" t="s">
         <v>39</v>
@@ -9623,12 +9626,12 @@
         <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -9640,29 +9643,29 @@
         <v>43</v>
       </c>
       <c r="F85" t="s">
-        <v>316</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
       </c>
       <c r="D86" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E86" t="s">
         <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>271</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C87" t="s">
         <v>39</v>
@@ -9674,12 +9677,12 @@
         <v>43</v>
       </c>
       <c r="F87" t="s">
-        <v>343</v>
+        <v>280</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C88" t="s">
         <v>39</v>
@@ -9696,7 +9699,7 @@
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C89" t="s">
         <v>39</v>
@@ -9708,12 +9711,12 @@
         <v>43</v>
       </c>
       <c r="F89" t="s">
-        <v>280</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C90" t="s">
         <v>39</v>
@@ -9725,12 +9728,12 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>108</v>
+        <v>280</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C91" t="s">
         <v>39</v>
@@ -9742,15 +9745,15 @@
         <v>43</v>
       </c>
       <c r="F91" t="s">
-        <v>280</v>
+        <v>345</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D92" t="s">
         <v>47</v>
@@ -9759,63 +9762,63 @@
         <v>43</v>
       </c>
       <c r="F92" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C93" t="s">
         <v>120</v>
       </c>
       <c r="D93" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E93" t="s">
         <v>43</v>
       </c>
       <c r="F93" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D94" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E94" t="s">
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>349</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C95" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="D95" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E95" t="s">
         <v>43</v>
       </c>
       <c r="F95" t="s">
-        <v>74</v>
+        <v>353</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C96" t="s">
         <v>120</v>
@@ -9827,29 +9830,29 @@
         <v>43</v>
       </c>
       <c r="F96" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C97" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D97" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E97" t="s">
         <v>43</v>
       </c>
       <c r="F97" t="s">
-        <v>343</v>
+        <v>74</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C98" t="s">
         <v>40</v>
@@ -9861,12 +9864,12 @@
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>74</v>
+        <v>795</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C99" t="s">
         <v>40</v>
@@ -9878,49 +9881,49 @@
         <v>43</v>
       </c>
       <c r="F99" t="s">
-        <v>795</v>
+        <v>378</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>369</v>
+        <v>991</v>
       </c>
       <c r="C100" t="s">
         <v>40</v>
       </c>
       <c r="D100" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E100" t="s">
         <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>378</v>
+        <v>993</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="D101" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E101" t="s">
         <v>43</v>
       </c>
       <c r="F101" t="s">
-        <v>993</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>994</v>
+        <v>1041</v>
       </c>
       <c r="C102" t="s">
-        <v>281</v>
+        <v>40</v>
       </c>
       <c r="D102" t="s">
         <v>42</v>
@@ -9929,12 +9932,12 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>1040</v>
+        <v>378</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C103" t="s">
         <v>40</v>
@@ -9946,12 +9949,12 @@
         <v>43</v>
       </c>
       <c r="F103" t="s">
-        <v>378</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C104" t="s">
         <v>40</v>
@@ -9963,12 +9966,12 @@
         <v>43</v>
       </c>
       <c r="F104" t="s">
-        <v>74</v>
+        <v>378</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C105" t="s">
         <v>40</v>
@@ -9980,29 +9983,29 @@
         <v>43</v>
       </c>
       <c r="F105" t="s">
-        <v>378</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>1044</v>
+        <v>1064</v>
       </c>
       <c r="C106" t="s">
         <v>40</v>
       </c>
       <c r="D106" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E106" t="s">
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>1060</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>1064</v>
+        <v>1072</v>
       </c>
       <c r="C107" t="s">
         <v>40</v>
@@ -10014,29 +10017,29 @@
         <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>1066</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>1072</v>
+        <v>1080</v>
       </c>
       <c r="C108" t="s">
         <v>40</v>
       </c>
       <c r="D108" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E108" t="s">
         <v>43</v>
       </c>
       <c r="F108" t="s">
-        <v>1075</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>1080</v>
+        <v>1104</v>
       </c>
       <c r="C109" t="s">
         <v>40</v>
@@ -10048,12 +10051,12 @@
         <v>43</v>
       </c>
       <c r="F109" t="s">
-        <v>1193</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>1104</v>
+        <v>1125</v>
       </c>
       <c r="C110" t="s">
         <v>40</v>
@@ -10065,46 +10068,46 @@
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>1121</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>1125</v>
+        <v>1164</v>
       </c>
       <c r="C111" t="s">
         <v>40</v>
       </c>
       <c r="D111" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E111" t="s">
         <v>43</v>
       </c>
       <c r="F111" t="s">
-        <v>1151</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>1164</v>
+        <v>1186</v>
       </c>
       <c r="C112" t="s">
         <v>40</v>
       </c>
       <c r="D112" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E112" t="s">
         <v>43</v>
       </c>
       <c r="F112" t="s">
-        <v>1173</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>1186</v>
+        <v>1229</v>
       </c>
       <c r="C113" t="s">
         <v>40</v>
@@ -10116,26 +10119,10 @@
         <v>43</v>
       </c>
       <c r="F113" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="B114" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C114" t="s">
-        <v>40</v>
-      </c>
-      <c r="D114" t="s">
-        <v>42</v>
-      </c>
-      <c r="E114" t="s">
-        <v>43</v>
-      </c>
-      <c r="F114" t="s">
         <v>1236</v>
       </c>
     </row>
+    <row r="114"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>